<commit_message>
scraped data from figures using Fiji
</commit_message>
<xml_diff>
--- a/data/scrapedExcel/egret_SS.xlsx
+++ b/data/scrapedExcel/egret_SS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\my_repo_dir\egret\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\my_repo_dir\egret\data\scrapedExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED4C768C-BBDF-4E10-B80D-870D7196A20C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D2DD337-4349-4B49-BA85-F35FFB7CCE5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4530,23 +4530,21 @@
   <dimension ref="A1:AS1305"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C1295" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AJ1308" sqref="AJ1308"/>
+      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="14.83203125" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
     <col min="4" max="4" width="10.4140625" customWidth="1"/>
     <col min="5" max="5" width="14.83203125" customWidth="1"/>
     <col min="6" max="6" width="8.25" customWidth="1"/>
     <col min="7" max="7" width="20.83203125" customWidth="1"/>
-    <col min="23" max="23" width="10.83203125" style="5"/>
-    <col min="25" max="25" width="10.83203125" style="5"/>
+    <col min="23" max="23" width="10.6640625" style="5"/>
+    <col min="25" max="25" width="10.6640625" style="5"/>
     <col min="36" max="36" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>